<commit_message>
Recalcular PVE y nombre columna industrial masivo
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.2 Plantilla_Eficiencia_energetica_industrial_caldera (retrofit).xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.2 Plantilla_Eficiencia_energetica_industrial_caldera (retrofit).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Web Dinamico 2\MRVMinem\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D5D896-44C9-4E6F-B1BE-61571B0E3DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F62A9E-B771-47F4-A669-79046F8993DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4B859084-2846-437A-9A39-CE5A20A8C627}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{4B859084-2846-437A-9A39-CE5A20A8C627}"/>
   </bookViews>
   <sheets>
     <sheet name="Energetica Industrial Caldera" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Año</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Volumen de combustible consumido por la caldera actual. En caso de combustibles: diesel y residual se debe usar galones y para gas natural en m3. Ingrese su dato.</t>
+  </si>
+  <si>
+    <t>Combustible (linea base y acción)</t>
   </si>
 </sst>
 </file>
@@ -682,14 +685,14 @@
   <dimension ref="A1:F312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" customWidth="1"/>
@@ -703,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>13</v>
@@ -5066,7 +5069,7 @@
       <c r="B312" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="R4DLD1CAM5Lg5LvvsKiGnq8xz2BtRjfgMy9yD6GHvVq/S0ZJ6E0nd9KFTDZp19a64f3FvMWn8+a/SGnt52VNAQ==" saltValue="ePkKp7Y261UTlH52slHM8Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="L/xz/uCKhqQUSHzltkz/hCrPpiEM1x5zAW8lRomw1NWZt22vr+eFQGlYy8Bg5wYB4YM9/WxkO7TY6KEYA+tAIA==" saltValue="i8UKpRdaLvrq1ncCT9iIog==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A2:F2"/>
   </mergeCells>

</xml_diff>